<commit_message>
CORRECCIONES DE HORARIO Y VALIDACIÓN DE ASISTENCIA
</commit_message>
<xml_diff>
--- a/ejemplo5.xlsx
+++ b/ejemplo5.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>Viernes</t>
   </si>
@@ -95,9 +95,6 @@
     <t>03IA</t>
   </si>
   <si>
-    <t>14:00</t>
-  </si>
-  <si>
     <t>04IB</t>
   </si>
   <si>
@@ -140,22 +137,34 @@
     <t>00:00</t>
   </si>
   <si>
+    <t>EC1</t>
+  </si>
+  <si>
+    <t>EC2</t>
+  </si>
+  <si>
+    <t>EC4</t>
+  </si>
+  <si>
+    <t>EA1</t>
+  </si>
+  <si>
+    <t>EA2</t>
+  </si>
+  <si>
+    <t>EB1</t>
+  </si>
+  <si>
+    <t>EB2</t>
+  </si>
+  <si>
+    <t>EB3</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
     <t>01:00</t>
-  </si>
-  <si>
-    <t>EC1</t>
-  </si>
-  <si>
-    <t>EC2</t>
-  </si>
-  <si>
-    <t>AC3</t>
-  </si>
-  <si>
-    <t>EC4</t>
-  </si>
-  <si>
-    <t>EC3</t>
   </si>
 </sst>
 </file>
@@ -477,44 +486,44 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -534,7 +543,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
@@ -557,7 +566,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -580,7 +589,7 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -588,22 +597,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -611,7 +620,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -620,13 +629,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -649,7 +658,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -672,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
@@ -695,7 +704,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -718,7 +727,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -729,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -741,34 +750,15 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>